<commit_message>
Add ingredient recipe routes and schema; enhance ingredient creation service
</commit_message>
<xml_diff>
--- a/RESSOURCES/ARTICLES/DB_ARTICLES.xlsx
+++ b/RESSOURCES/ARTICLES/DB_ARTICLES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\ARTICLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\_apps\DIVISIO\RESSOURCES\ARTICLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E055B9-44C8-4167-8A03-0DF68499FB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AB87BE-05AB-4D9F-9020-23AC3505A8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="30180" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -6581,8 +6581,8 @@
   <dimension ref="A1:G900"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I360" sqref="I360"/>
+      <pane ySplit="1" topLeftCell="A450" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H877" sqref="H877"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12872,7 +12872,7 @@
         <v>2064</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="3" t="s">
         <v>1477</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
         <v>1478</v>
       </c>
@@ -12908,7 +12908,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
         <v>1479</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
         <v>1480</v>
       </c>
@@ -12944,7 +12944,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
         <v>1481</v>
       </c>
@@ -12962,7 +12962,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
         <v>1482</v>
       </c>
@@ -12980,7 +12980,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
         <v>1483</v>
       </c>
@@ -12998,7 +12998,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
         <v>1484</v>
       </c>
@@ -13016,7 +13016,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
         <v>1485</v>
       </c>
@@ -13034,7 +13034,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
         <v>1486</v>
       </c>
@@ -13052,7 +13052,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
         <v>1487</v>
       </c>
@@ -13070,7 +13070,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="s">
         <v>1488</v>
       </c>
@@ -13088,7 +13088,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="3" t="s">
         <v>1489</v>
       </c>
@@ -13106,7 +13106,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="3" t="s">
         <v>1490</v>
       </c>
@@ -13124,7 +13124,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="3" t="s">
         <v>1491</v>
       </c>
@@ -13142,7 +13142,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="3" t="s">
         <v>1492</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="3" t="s">
         <v>1493</v>
       </c>
@@ -13178,7 +13178,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="3" t="s">
         <v>1494</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="3" t="s">
         <v>1495</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="3" t="s">
         <v>1496</v>
       </c>
@@ -13232,7 +13232,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="3" t="s">
         <v>1497</v>
       </c>
@@ -13250,7 +13250,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="3" t="s">
         <v>1498</v>
       </c>
@@ -13268,7 +13268,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="3" t="s">
         <v>1499</v>
       </c>
@@ -14922,7 +14922,7 @@
         <v>2064</v>
       </c>
     </row>
-    <row r="455" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455" s="3" t="s">
         <v>1588</v>
       </c>
@@ -14976,7 +14976,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="458" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
         <v>1591</v>
       </c>
@@ -22784,7 +22784,7 @@
       <c r="D871" s="5">
         <v>1</v>
       </c>
-      <c r="E871" s="5" t="s">
+      <c r="E871" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F871" s="5" t="s">
@@ -22801,7 +22801,7 @@
       <c r="D872" s="5">
         <v>1</v>
       </c>
-      <c r="E872" s="5" t="s">
+      <c r="E872" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F872" s="5" t="s">
@@ -22818,7 +22818,7 @@
       <c r="D873" s="5">
         <v>1</v>
       </c>
-      <c r="E873" s="5" t="s">
+      <c r="E873" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F873" s="5" t="s">
@@ -22835,7 +22835,7 @@
       <c r="D874" s="5">
         <v>1</v>
       </c>
-      <c r="E874" s="5" t="s">
+      <c r="E874" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F874" s="5" t="s">
@@ -22852,14 +22852,14 @@
       <c r="D875" s="5">
         <v>1</v>
       </c>
-      <c r="E875" s="5" t="s">
+      <c r="E875" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F875" s="5" t="s">
         <v>1999</v>
       </c>
     </row>
-    <row r="876" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A876" s="5" t="s">
         <v>2006</v>
       </c>
@@ -22876,7 +22876,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="877" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A877" s="5" t="s">
         <v>2007</v>
       </c>
@@ -22893,7 +22893,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="878" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A878" s="5" t="s">
         <v>2008</v>
       </c>
@@ -22910,7 +22910,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="879" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A879" s="5" t="s">
         <v>2009</v>
       </c>
@@ -22927,7 +22927,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="880" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A880" s="5" t="s">
         <v>2010</v>
       </c>
@@ -22944,7 +22944,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="881" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A881" s="5" t="s">
         <v>2011</v>
       </c>
@@ -22961,7 +22961,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="882" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A882" s="5" t="s">
         <v>2012</v>
       </c>
@@ -22978,7 +22978,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="883" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A883" s="5" t="s">
         <v>2013</v>
       </c>
@@ -23005,7 +23005,7 @@
       <c r="D884" s="5">
         <v>1</v>
       </c>
-      <c r="E884" s="5" t="s">
+      <c r="E884" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F884" s="5" t="s">
@@ -23022,7 +23022,7 @@
       <c r="D885" s="5">
         <v>1</v>
       </c>
-      <c r="E885" s="5" t="s">
+      <c r="E885" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F885" s="5" t="s">
@@ -23039,7 +23039,7 @@
       <c r="D886" s="5">
         <v>1</v>
       </c>
-      <c r="E886" s="5" t="s">
+      <c r="E886" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F886" s="5" t="s">
@@ -23056,7 +23056,7 @@
       <c r="D887" s="5">
         <v>1</v>
       </c>
-      <c r="E887" s="5" t="s">
+      <c r="E887" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F887" s="5" t="s">
@@ -23073,7 +23073,7 @@
       <c r="D888" s="5">
         <v>1</v>
       </c>
-      <c r="E888" s="5" t="s">
+      <c r="E888" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F888" s="5" t="s">
@@ -23090,14 +23090,14 @@
       <c r="D889" s="5">
         <v>1</v>
       </c>
-      <c r="E889" s="5" t="s">
+      <c r="E889" s="3" t="s">
         <v>1131</v>
       </c>
       <c r="F889" s="5" t="s">
         <v>1999</v>
       </c>
     </row>
-    <row r="890" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A890" s="5" t="s">
         <v>2014</v>
       </c>
@@ -23114,7 +23114,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="891" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A891" s="5" t="s">
         <v>2024</v>
       </c>
@@ -23131,7 +23131,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="892" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A892" s="5" t="s">
         <v>2026</v>
       </c>
@@ -23148,7 +23148,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="893" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A893" s="5" t="s">
         <v>2028</v>
       </c>
@@ -23165,7 +23165,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="894" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A894" s="5" t="s">
         <v>2030</v>
       </c>
@@ -23182,7 +23182,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="895" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A895" s="5" t="s">
         <v>2032</v>
       </c>
@@ -23199,7 +23199,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="896" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A896" s="5" t="s">
         <v>2034</v>
       </c>
@@ -23216,7 +23216,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="897" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A897" s="5" t="s">
         <v>2036</v>
       </c>
@@ -23233,7 +23233,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="898" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A898" s="2" t="s">
         <v>2038</v>
       </c>
@@ -23250,7 +23250,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="899" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A899" s="2" t="s">
         <v>2040</v>
       </c>
@@ -23267,7 +23267,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="900" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A900" s="2" t="s">
         <v>2042</v>
       </c>
@@ -23286,9 +23286,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F900" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="5">
+    <filterColumn colId="4">
       <filters>
-        <filter val="G"/>
+        <filter val="Semi-fini"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>